<commit_message>
Made priority work by inversing Order
</commit_message>
<xml_diff>
--- a/src/EPPlusTest/Workbooks/CondtionalFormattingHtmlExport.xlsx
+++ b/src/EPPlusTest/Workbooks/CondtionalFormattingHtmlExport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kod\EPPlusSoftware\EPPlus7\EPPlus\src\EPPlusTest\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OssianEdström\Documents\Epplus_Repos\HtmlEpplusBugs\EPPlus\src\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A09307E-496F-4F9E-A79A-5B38E77CF094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099FB84-CF21-4F24-9696-0473F96EBAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2235" yWindow="1470" windowWidth="26565" windowHeight="14010" xr2:uid="{9ABB0F2C-23F3-4ECD-B4BD-6FCFC6139632}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9ABB0F2C-23F3-4ECD-B4BD-6FCFC6139632}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,13 +89,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,13 +132,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <u/>
+        <color theme="5"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -517,139 +602,253 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44ED580D-FE3B-4C7F-A4B8-AA0A6702F05A}">
-  <dimension ref="B2:C15"/>
+  <dimension ref="B2:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>ROW()</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>ROW()</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>ROW()</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>ROW()</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>ROW()</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E8" s="3">
+        <f>ROW()</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <f>ROW()</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>ROW()</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <f>ROW()</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>12</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>ROW()</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>13</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>ROW()</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>ROW()</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>15</v>
       </c>
+      <c r="E15">
+        <f>ROW()</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <f>ROW()</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <f>ROW()</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <f>ROW()</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <f>ROW()</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f>ROW()</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <f>ROW()</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <f>ROW()</f>
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B15">
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="10" priority="9">
       <formula>$B2&lt;7</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="4" priority="5" rank="10"/>
-    <cfRule type="top10" dxfId="3" priority="6" percent="1" rank="25"/>
+    <cfRule type="top10" dxfId="9" priority="10" rank="10"/>
+    <cfRule type="top10" dxfId="8" priority="11" percent="1" rank="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C15">
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",C2)))</formula>
     </cfRule>
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="containsBlanks" dxfId="0" priority="7">
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="containsBlanks" dxfId="5" priority="12">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E22">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>IF(E2 = 10,TRUE,FALSE)</formula>
+    </cfRule>
+    <cfRule type="top10" dxfId="3" priority="2" bottom="1" rank="2"/>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
+      <formula>2</formula>
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="between">
+      <formula>5</formula>
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="uniqueValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>